<commit_message>
M1/M2 Table Deleted from FODO
</commit_message>
<xml_diff>
--- a/Form_FODO_SurveyReport.xlsx
+++ b/Form_FODO_SurveyReport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\APS-U\Assembly-Survey-Report-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Documents\Assembly-Survey-Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56F82EE-DBFA-4CDD-B012-43F40CC3B32A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7079D8-0B7F-49CC-962F-9C25C5EA835D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>APS Upgrade</t>
   </si>
@@ -85,9 +85,6 @@
     <t>ABS Max</t>
   </si>
   <si>
-    <t>NOTE:</t>
-  </si>
-  <si>
     <t>Report created:</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
   </si>
   <si>
     <t>FODO_###</t>
-  </si>
-  <si>
-    <t>M1/M2 data is not included in the statistics reported above.</t>
   </si>
 </sst>
 </file>
@@ -194,7 +188,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,20 +207,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFEDCD6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="38">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -411,37 +393,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -548,154 +499,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -730,7 +533,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -822,13 +625,13 @@
       <alignment horizontal="right" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="3"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -837,22 +640,13 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -864,28 +658,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -895,24 +668,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="3"/>
@@ -926,19 +681,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="3"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -947,20 +702,35 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1312,7 +1082,7 @@
   <dimension ref="B1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1324,59 +1094,59 @@
   <sheetData>
     <row r="1" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="48" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B3" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="55"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B4" s="55" t="s">
+      <c r="B3" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="55"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B5" s="55" t="s">
+      <c r="C3" s="45"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B4" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="55"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B6" s="55" t="s">
+      <c r="C4" s="45"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B5" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="56"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B7" s="55" t="s">
+      <c r="C5" s="45"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B6" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="55"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B8" s="55" t="s">
+      <c r="C6" s="46"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B7" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="56"/>
+      <c r="C7" s="45"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B8" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="46"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="47" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1422,7 +1192,7 @@
       <c r="B17" s="20"/>
       <c r="C17" s="21"/>
       <c r="D17" s="22"/>
-      <c r="G17" s="68"/>
+      <c r="G17" s="52"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B18" s="20"/>
@@ -1467,21 +1237,21 @@
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
       <c r="E25" s="39"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="70"/>
-      <c r="H25" s="71"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="55"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B26" s="44"/>
+      <c r="B26" s="41"/>
       <c r="C26" s="11"/>
       <c r="D26" s="12"/>
       <c r="E26" s="33"/>
-      <c r="F26" s="72"/>
-      <c r="G26" s="65"/>
-      <c r="H26" s="73"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="57"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B27" s="45"/>
+      <c r="B27" s="42"/>
       <c r="C27" s="13"/>
       <c r="D27" s="14"/>
       <c r="E27" s="34"/>
@@ -1490,7 +1260,7 @@
       <c r="H27" s="38"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B28" s="45"/>
+      <c r="B28" s="42"/>
       <c r="C28" s="13"/>
       <c r="D28" s="14"/>
       <c r="E28" s="34"/>
@@ -1499,7 +1269,7 @@
       <c r="H28" s="38"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B29" s="45"/>
+      <c r="B29" s="42"/>
       <c r="C29" s="13"/>
       <c r="D29" s="14"/>
       <c r="E29" s="34"/>
@@ -1508,7 +1278,7 @@
       <c r="H29" s="38"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B30" s="45"/>
+      <c r="B30" s="42"/>
       <c r="C30" s="13"/>
       <c r="D30" s="14"/>
       <c r="E30" s="34"/>
@@ -1517,7 +1287,7 @@
       <c r="H30" s="38"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B31" s="45"/>
+      <c r="B31" s="42"/>
       <c r="C31" s="13"/>
       <c r="D31" s="14"/>
       <c r="E31" s="34"/>
@@ -1526,7 +1296,7 @@
       <c r="H31" s="38"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B32" s="45"/>
+      <c r="B32" s="42"/>
       <c r="C32" s="13"/>
       <c r="D32" s="14"/>
       <c r="E32" s="34"/>
@@ -1535,13 +1305,13 @@
       <c r="H32" s="38"/>
     </row>
     <row r="33" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="46"/>
+      <c r="B33" s="43"/>
       <c r="C33" s="15"/>
       <c r="D33" s="16"/>
       <c r="E33" s="35"/>
-      <c r="F33" s="74"/>
-      <c r="G33" s="75"/>
-      <c r="H33" s="76"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="60"/>
     </row>
     <row r="34" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B34" s="5"/>
@@ -1568,15 +1338,15 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F35" s="65" t="e">
+      <c r="F35" s="49" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G35" s="65" t="e">
+      <c r="G35" s="49" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H35" s="65" t="e">
+      <c r="H35" s="49" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -1597,15 +1367,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F36" s="66">
+      <c r="F36" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G36" s="66">
+      <c r="G36" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H36" s="66">
+      <c r="H36" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1626,74 +1396,48 @@
         <f t="array" ref="E37">MAX(ABS(E26:E33))</f>
         <v>0</v>
       </c>
-      <c r="F37" s="67" cm="1">
+      <c r="F37" s="51" cm="1">
         <f t="array" ref="F37">MAX(ABS(F26:F33))</f>
         <v>0</v>
       </c>
-      <c r="G37" s="67" cm="1">
+      <c r="G37" s="51" cm="1">
         <f t="array" ref="G37">MAX(ABS(G26:G33))</f>
         <v>0</v>
       </c>
-      <c r="H37" s="67" cm="1">
+      <c r="H37" s="51" cm="1">
         <f t="array" ref="H37">MAX(ABS(H26:H33))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="40" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="50">
-        <f t="shared" ref="B40:H40" si="2">B25</f>
-        <v>0</v>
-      </c>
-      <c r="C40" s="48">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D40" s="53">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E40" s="48">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F40" s="47">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G40" s="53">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H40" s="49">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B40" s="62"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="62"/>
+      <c r="E40" s="62"/>
+      <c r="F40" s="62"/>
+      <c r="G40" s="62"/>
+      <c r="H40" s="62"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B41" s="54"/>
-      <c r="C41" s="59"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="62"/>
-      <c r="G41" s="63"/>
-      <c r="H41" s="64"/>
-    </row>
-    <row r="42" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="52" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="D42" s="78"/>
-      <c r="E42" s="79"/>
-      <c r="F42" s="41"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="43"/>
+      <c r="B41" s="63"/>
+      <c r="C41" s="64"/>
+      <c r="D41" s="64"/>
+      <c r="E41" s="65"/>
+      <c r="F41" s="66"/>
+      <c r="G41" s="66"/>
+      <c r="H41" s="66"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B42" s="67"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="69"/>
+      <c r="E42" s="69"/>
+      <c r="F42" s="68"/>
+      <c r="G42" s="68"/>
+      <c r="H42" s="68"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B43" s="51"/>
+      <c r="B43" s="44"/>
       <c r="C43" s="40"/>
       <c r="D43" s="40"/>
       <c r="E43" s="40"/>
@@ -1711,9 +1455,6 @@
       <c r="H44" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C42:E42"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="86" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -2457,11 +2198,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="210" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="80"/>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
+      <c r="A1" s="61"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="27"/>
@@ -2590,21 +2331,21 @@
       <c r="B23" s="25"/>
     </row>
     <row r="24" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="80"/>
-      <c r="B24" s="80"/>
-      <c r="C24" s="80"/>
-      <c r="D24" s="80"/>
-      <c r="E24" s="80"/>
-      <c r="F24" s="80"/>
-      <c r="G24" s="80"/>
-      <c r="H24" s="80"/>
-      <c r="I24" s="80"/>
-      <c r="J24" s="80"/>
-      <c r="K24" s="80"/>
-      <c r="L24" s="80"/>
-      <c r="M24" s="80"/>
-      <c r="N24" s="80"/>
-      <c r="O24" s="80"/>
+      <c r="A24" s="61"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="61"/>
+      <c r="K24" s="61"/>
+      <c r="L24" s="61"/>
+      <c r="M24" s="61"/>
+      <c r="N24" s="61"/>
+      <c r="O24" s="61"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="27"/>
@@ -3712,11 +3453,11 @@
       <c r="O89" s="25"/>
     </row>
     <row r="90" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="80"/>
-      <c r="B90" s="80"/>
-      <c r="C90" s="80"/>
-      <c r="D90" s="80"/>
-      <c r="E90" s="80"/>
+      <c r="A90" s="61"/>
+      <c r="B90" s="61"/>
+      <c r="C90" s="61"/>
+      <c r="D90" s="61"/>
+      <c r="E90" s="61"/>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A91" s="27"/>
@@ -3845,21 +3586,21 @@
       <c r="B112" s="25"/>
     </row>
     <row r="113" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="80"/>
-      <c r="B113" s="80"/>
-      <c r="C113" s="80"/>
-      <c r="D113" s="80"/>
-      <c r="E113" s="80"/>
-      <c r="F113" s="80"/>
-      <c r="G113" s="80"/>
-      <c r="H113" s="80"/>
-      <c r="I113" s="80"/>
-      <c r="J113" s="80"/>
-      <c r="K113" s="80"/>
-      <c r="L113" s="80"/>
-      <c r="M113" s="80"/>
-      <c r="N113" s="80"/>
-      <c r="O113" s="80"/>
+      <c r="A113" s="61"/>
+      <c r="B113" s="61"/>
+      <c r="C113" s="61"/>
+      <c r="D113" s="61"/>
+      <c r="E113" s="61"/>
+      <c r="F113" s="61"/>
+      <c r="G113" s="61"/>
+      <c r="H113" s="61"/>
+      <c r="I113" s="61"/>
+      <c r="J113" s="61"/>
+      <c r="K113" s="61"/>
+      <c r="L113" s="61"/>
+      <c r="M113" s="61"/>
+      <c r="N113" s="61"/>
+      <c r="O113" s="61"/>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A114" s="27"/>
@@ -4015,11 +3756,11 @@
       <c r="O122" s="25"/>
     </row>
     <row r="123" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="80"/>
-      <c r="B123" s="80"/>
-      <c r="C123" s="80"/>
-      <c r="D123" s="80"/>
-      <c r="E123" s="80"/>
+      <c r="A123" s="61"/>
+      <c r="B123" s="61"/>
+      <c r="C123" s="61"/>
+      <c r="D123" s="61"/>
+      <c r="E123" s="61"/>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A124" s="27"/>
@@ -4148,21 +3889,21 @@
       <c r="B145" s="25"/>
     </row>
     <row r="146" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A146" s="80"/>
-      <c r="B146" s="80"/>
-      <c r="C146" s="80"/>
-      <c r="D146" s="80"/>
-      <c r="E146" s="80"/>
-      <c r="F146" s="80"/>
-      <c r="G146" s="80"/>
-      <c r="H146" s="80"/>
-      <c r="I146" s="80"/>
-      <c r="J146" s="80"/>
-      <c r="K146" s="80"/>
-      <c r="L146" s="80"/>
-      <c r="M146" s="80"/>
-      <c r="N146" s="80"/>
-      <c r="O146" s="80"/>
+      <c r="A146" s="61"/>
+      <c r="B146" s="61"/>
+      <c r="C146" s="61"/>
+      <c r="D146" s="61"/>
+      <c r="E146" s="61"/>
+      <c r="F146" s="61"/>
+      <c r="G146" s="61"/>
+      <c r="H146" s="61"/>
+      <c r="I146" s="61"/>
+      <c r="J146" s="61"/>
+      <c r="K146" s="61"/>
+      <c r="L146" s="61"/>
+      <c r="M146" s="61"/>
+      <c r="N146" s="61"/>
+      <c r="O146" s="61"/>
     </row>
     <row r="147" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A147" s="27"/>
@@ -4335,11 +4076,11 @@
       <c r="O156" s="25"/>
     </row>
     <row r="157" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A157" s="80"/>
-      <c r="B157" s="80"/>
-      <c r="C157" s="80"/>
-      <c r="D157" s="80"/>
-      <c r="E157" s="80"/>
+      <c r="A157" s="61"/>
+      <c r="B157" s="61"/>
+      <c r="C157" s="61"/>
+      <c r="D157" s="61"/>
+      <c r="E157" s="61"/>
     </row>
     <row r="158" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A158" s="27"/>
@@ -4468,21 +4209,21 @@
       <c r="B179" s="25"/>
     </row>
     <row r="180" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A180" s="80"/>
-      <c r="B180" s="80"/>
-      <c r="C180" s="80"/>
-      <c r="D180" s="80"/>
-      <c r="E180" s="80"/>
-      <c r="F180" s="80"/>
-      <c r="G180" s="80"/>
-      <c r="H180" s="80"/>
-      <c r="I180" s="80"/>
-      <c r="J180" s="80"/>
-      <c r="K180" s="80"/>
-      <c r="L180" s="80"/>
-      <c r="M180" s="80"/>
-      <c r="N180" s="80"/>
-      <c r="O180" s="80"/>
+      <c r="A180" s="61"/>
+      <c r="B180" s="61"/>
+      <c r="C180" s="61"/>
+      <c r="D180" s="61"/>
+      <c r="E180" s="61"/>
+      <c r="F180" s="61"/>
+      <c r="G180" s="61"/>
+      <c r="H180" s="61"/>
+      <c r="I180" s="61"/>
+      <c r="J180" s="61"/>
+      <c r="K180" s="61"/>
+      <c r="L180" s="61"/>
+      <c r="M180" s="61"/>
+      <c r="N180" s="61"/>
+      <c r="O180" s="61"/>
     </row>
     <row r="181" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A181" s="27"/>
@@ -4621,11 +4362,11 @@
       <c r="O188" s="25"/>
     </row>
     <row r="189" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A189" s="80"/>
-      <c r="B189" s="80"/>
-      <c r="C189" s="80"/>
-      <c r="D189" s="80"/>
-      <c r="E189" s="80"/>
+      <c r="A189" s="61"/>
+      <c r="B189" s="61"/>
+      <c r="C189" s="61"/>
+      <c r="D189" s="61"/>
+      <c r="E189" s="61"/>
     </row>
     <row r="190" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A190" s="27"/>
@@ -4754,21 +4495,21 @@
       <c r="B211" s="25"/>
     </row>
     <row r="212" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A212" s="80"/>
-      <c r="B212" s="80"/>
-      <c r="C212" s="80"/>
-      <c r="D212" s="80"/>
-      <c r="E212" s="80"/>
-      <c r="F212" s="80"/>
-      <c r="G212" s="80"/>
-      <c r="H212" s="80"/>
-      <c r="I212" s="80"/>
-      <c r="J212" s="80"/>
-      <c r="K212" s="80"/>
-      <c r="L212" s="80"/>
-      <c r="M212" s="80"/>
-      <c r="N212" s="80"/>
-      <c r="O212" s="80"/>
+      <c r="A212" s="61"/>
+      <c r="B212" s="61"/>
+      <c r="C212" s="61"/>
+      <c r="D212" s="61"/>
+      <c r="E212" s="61"/>
+      <c r="F212" s="61"/>
+      <c r="G212" s="61"/>
+      <c r="H212" s="61"/>
+      <c r="I212" s="61"/>
+      <c r="J212" s="61"/>
+      <c r="K212" s="61"/>
+      <c r="L212" s="61"/>
+      <c r="M212" s="61"/>
+      <c r="N212" s="61"/>
+      <c r="O212" s="61"/>
     </row>
     <row r="213" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A213" s="27"/>
@@ -4924,11 +4665,11 @@
       <c r="O221" s="25"/>
     </row>
     <row r="222" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A222" s="80"/>
-      <c r="B222" s="80"/>
-      <c r="C222" s="80"/>
-      <c r="D222" s="80"/>
-      <c r="E222" s="80"/>
+      <c r="A222" s="61"/>
+      <c r="B222" s="61"/>
+      <c r="C222" s="61"/>
+      <c r="D222" s="61"/>
+      <c r="E222" s="61"/>
     </row>
     <row r="223" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A223" s="27"/>
@@ -5057,21 +4798,21 @@
       <c r="B244" s="25"/>
     </row>
     <row r="245" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A245" s="80"/>
-      <c r="B245" s="80"/>
-      <c r="C245" s="80"/>
-      <c r="D245" s="80"/>
-      <c r="E245" s="80"/>
-      <c r="F245" s="80"/>
-      <c r="G245" s="80"/>
-      <c r="H245" s="80"/>
-      <c r="I245" s="80"/>
-      <c r="J245" s="80"/>
-      <c r="K245" s="80"/>
-      <c r="L245" s="80"/>
-      <c r="M245" s="80"/>
-      <c r="N245" s="80"/>
-      <c r="O245" s="80"/>
+      <c r="A245" s="61"/>
+      <c r="B245" s="61"/>
+      <c r="C245" s="61"/>
+      <c r="D245" s="61"/>
+      <c r="E245" s="61"/>
+      <c r="F245" s="61"/>
+      <c r="G245" s="61"/>
+      <c r="H245" s="61"/>
+      <c r="I245" s="61"/>
+      <c r="J245" s="61"/>
+      <c r="K245" s="61"/>
+      <c r="L245" s="61"/>
+      <c r="M245" s="61"/>
+      <c r="N245" s="61"/>
+      <c r="O245" s="61"/>
     </row>
     <row r="246" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A246" s="27"/>
@@ -5227,11 +4968,11 @@
       <c r="O254" s="25"/>
     </row>
     <row r="255" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A255" s="80"/>
-      <c r="B255" s="80"/>
-      <c r="C255" s="80"/>
-      <c r="D255" s="80"/>
-      <c r="E255" s="80"/>
+      <c r="A255" s="61"/>
+      <c r="B255" s="61"/>
+      <c r="C255" s="61"/>
+      <c r="D255" s="61"/>
+      <c r="E255" s="61"/>
     </row>
     <row r="256" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A256" s="27"/>
@@ -5360,21 +5101,21 @@
       <c r="B277" s="25"/>
     </row>
     <row r="278" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A278" s="80"/>
-      <c r="B278" s="80"/>
-      <c r="C278" s="80"/>
-      <c r="D278" s="80"/>
-      <c r="E278" s="80"/>
-      <c r="F278" s="80"/>
-      <c r="G278" s="80"/>
-      <c r="H278" s="80"/>
-      <c r="I278" s="80"/>
-      <c r="J278" s="80"/>
-      <c r="K278" s="80"/>
-      <c r="L278" s="80"/>
-      <c r="M278" s="80"/>
-      <c r="N278" s="80"/>
-      <c r="O278" s="80"/>
+      <c r="A278" s="61"/>
+      <c r="B278" s="61"/>
+      <c r="C278" s="61"/>
+      <c r="D278" s="61"/>
+      <c r="E278" s="61"/>
+      <c r="F278" s="61"/>
+      <c r="G278" s="61"/>
+      <c r="H278" s="61"/>
+      <c r="I278" s="61"/>
+      <c r="J278" s="61"/>
+      <c r="K278" s="61"/>
+      <c r="L278" s="61"/>
+      <c r="M278" s="61"/>
+      <c r="N278" s="61"/>
+      <c r="O278" s="61"/>
     </row>
     <row r="279" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A279" s="27"/>
@@ -5530,11 +5271,11 @@
       <c r="O287" s="25"/>
     </row>
     <row r="288" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A288" s="80"/>
-      <c r="B288" s="80"/>
-      <c r="C288" s="80"/>
-      <c r="D288" s="80"/>
-      <c r="E288" s="80"/>
+      <c r="A288" s="61"/>
+      <c r="B288" s="61"/>
+      <c r="C288" s="61"/>
+      <c r="D288" s="61"/>
+      <c r="E288" s="61"/>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A289" s="27"/>
@@ -5663,21 +5404,21 @@
       <c r="B310" s="25"/>
     </row>
     <row r="311" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A311" s="80"/>
-      <c r="B311" s="80"/>
-      <c r="C311" s="80"/>
-      <c r="D311" s="80"/>
-      <c r="E311" s="80"/>
-      <c r="F311" s="80"/>
-      <c r="G311" s="80"/>
-      <c r="H311" s="80"/>
-      <c r="I311" s="80"/>
-      <c r="J311" s="80"/>
-      <c r="K311" s="80"/>
-      <c r="L311" s="80"/>
-      <c r="M311" s="80"/>
-      <c r="N311" s="80"/>
-      <c r="O311" s="80"/>
+      <c r="A311" s="61"/>
+      <c r="B311" s="61"/>
+      <c r="C311" s="61"/>
+      <c r="D311" s="61"/>
+      <c r="E311" s="61"/>
+      <c r="F311" s="61"/>
+      <c r="G311" s="61"/>
+      <c r="H311" s="61"/>
+      <c r="I311" s="61"/>
+      <c r="J311" s="61"/>
+      <c r="K311" s="61"/>
+      <c r="L311" s="61"/>
+      <c r="M311" s="61"/>
+      <c r="N311" s="61"/>
+      <c r="O311" s="61"/>
     </row>
     <row r="312" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A312" s="27"/>
@@ -5833,11 +5574,11 @@
       <c r="O320" s="25"/>
     </row>
     <row r="321" spans="1:5" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A321" s="80"/>
-      <c r="B321" s="80"/>
-      <c r="C321" s="80"/>
-      <c r="D321" s="80"/>
-      <c r="E321" s="80"/>
+      <c r="A321" s="61"/>
+      <c r="B321" s="61"/>
+      <c r="C321" s="61"/>
+      <c r="D321" s="61"/>
+      <c r="E321" s="61"/>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A322" s="27"/>
@@ -5966,21 +5707,21 @@
       <c r="B343" s="25"/>
     </row>
     <row r="344" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A344" s="80"/>
-      <c r="B344" s="80"/>
-      <c r="C344" s="80"/>
-      <c r="D344" s="80"/>
-      <c r="E344" s="80"/>
-      <c r="F344" s="80"/>
-      <c r="G344" s="80"/>
-      <c r="H344" s="80"/>
-      <c r="I344" s="80"/>
-      <c r="J344" s="80"/>
-      <c r="K344" s="80"/>
-      <c r="L344" s="80"/>
-      <c r="M344" s="80"/>
-      <c r="N344" s="80"/>
-      <c r="O344" s="80"/>
+      <c r="A344" s="61"/>
+      <c r="B344" s="61"/>
+      <c r="C344" s="61"/>
+      <c r="D344" s="61"/>
+      <c r="E344" s="61"/>
+      <c r="F344" s="61"/>
+      <c r="G344" s="61"/>
+      <c r="H344" s="61"/>
+      <c r="I344" s="61"/>
+      <c r="J344" s="61"/>
+      <c r="K344" s="61"/>
+      <c r="L344" s="61"/>
+      <c r="M344" s="61"/>
+      <c r="N344" s="61"/>
+      <c r="O344" s="61"/>
     </row>
     <row r="345" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A345" s="27"/>
@@ -6137,11 +5878,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A24:O24"/>
-    <mergeCell ref="A90:E90"/>
-    <mergeCell ref="A113:O113"/>
-    <mergeCell ref="A123:E123"/>
     <mergeCell ref="A288:E288"/>
     <mergeCell ref="A311:O311"/>
     <mergeCell ref="A321:E321"/>
@@ -6155,6 +5891,11 @@
     <mergeCell ref="A245:O245"/>
     <mergeCell ref="A255:E255"/>
     <mergeCell ref="A278:O278"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A24:O24"/>
+    <mergeCell ref="A90:E90"/>
+    <mergeCell ref="A113:O113"/>
+    <mergeCell ref="A123:E123"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6813,16 +6554,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="165" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="80"/>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
+      <c r="A1" s="61"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="23"/>

</xml_diff>